<commit_message>
Initial Rmd script completed. Ready for further testing.
</commit_message>
<xml_diff>
--- a/data/DionexTest_raw.xlsx
+++ b/data/DionexTest_raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Dionex-HPLC-Data-Parser\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6028732E-755E-4F41-8A94-0C4F3975F225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A499FAA8-E604-4A58-B034-997693F8208C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="high8" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="142">
   <si>
     <t>Summary</t>
   </si>
@@ -438,6 +438,30 @@
   </si>
   <si>
     <t>phosphate</t>
+  </si>
+  <si>
+    <t>O220216h_D1:4</t>
+  </si>
+  <si>
+    <t>O210826h_D1:8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O210826h_D1:25 </t>
+  </si>
+  <si>
+    <t>S210826h_D1:10</t>
+  </si>
+  <si>
+    <t>J220216h_D1:2</t>
+  </si>
+  <si>
+    <t>O220216h_D1:10</t>
+  </si>
+  <si>
+    <t>CHECK_5.03</t>
+  </si>
+  <si>
+    <t>CHECK_0.2445</t>
   </si>
 </sst>
 </file>
@@ -458,7 +482,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,6 +492,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,12 +526,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,7 +818,7 @@
   <dimension ref="A1:BI54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4592,7 +4637,7 @@
   <dimension ref="A1:Z54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9639,7 +9684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C4C837-D6D6-4E78-8363-E905B8B703CC}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -9886,13 +9931,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4A690A-2088-4318-AF5D-5C228B4ACC23}">
   <dimension ref="A1:BI54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="11" max="11" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.3">
@@ -10486,7 +10532,7 @@
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
@@ -10560,7 +10606,7 @@
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C18">
@@ -10634,7 +10680,7 @@
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C19">
@@ -10708,7 +10754,7 @@
       <c r="A20">
         <v>6</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C20">
@@ -10782,7 +10828,7 @@
       <c r="A21">
         <v>7</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C21">
@@ -10856,7 +10902,7 @@
       <c r="A22">
         <v>8</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C22">
@@ -10930,7 +10976,7 @@
       <c r="A23">
         <v>9</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C23">
@@ -11004,7 +11050,7 @@
       <c r="A24">
         <v>10</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C24">
@@ -11078,7 +11124,7 @@
       <c r="A25">
         <v>11</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C25">
@@ -11152,7 +11198,7 @@
       <c r="A26">
         <v>12</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C26">
@@ -11226,7 +11272,7 @@
       <c r="A27">
         <v>13</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C27">
@@ -11374,8 +11420,8 @@
       <c r="A29">
         <v>15</v>
       </c>
-      <c r="B29" t="s">
-        <v>43</v>
+      <c r="B29" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="C29">
         <v>4.2439999999999998</v>
@@ -11399,7 +11445,7 @@
         <v>15</v>
       </c>
       <c r="K29" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="L29">
         <v>5.6609999999999996</v>
@@ -11423,7 +11469,7 @@
         <v>15</v>
       </c>
       <c r="T29" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="U29">
         <v>7.3339999999999996</v>
@@ -11460,8 +11506,8 @@
       <c r="A30">
         <v>16</v>
       </c>
-      <c r="B30" t="s">
-        <v>44</v>
+      <c r="B30" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="C30">
         <v>4.2439999999999998</v>
@@ -11485,7 +11531,7 @@
         <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="L30">
         <v>5.6669999999999998</v>
@@ -11509,7 +11555,7 @@
         <v>16</v>
       </c>
       <c r="T30" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="U30">
         <v>7.3540000000000001</v>
@@ -11964,8 +12010,8 @@
       <c r="A36">
         <v>22</v>
       </c>
-      <c r="B36" t="s">
-        <v>49</v>
+      <c r="B36" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="C36">
         <v>4.2469999999999999</v>
@@ -11989,7 +12035,7 @@
         <v>22</v>
       </c>
       <c r="K36" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="L36">
         <v>5.6609999999999996</v>
@@ -12013,7 +12059,7 @@
         <v>22</v>
       </c>
       <c r="T36" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="U36">
         <v>7.3639999999999999</v>
@@ -12128,8 +12174,8 @@
       <c r="A38">
         <v>24</v>
       </c>
-      <c r="B38" t="s">
-        <v>43</v>
+      <c r="B38" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="C38">
         <v>4.2409999999999997</v>
@@ -12153,7 +12199,7 @@
         <v>24</v>
       </c>
       <c r="K38" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="L38">
         <v>5.6609999999999996</v>
@@ -12177,7 +12223,7 @@
         <v>24</v>
       </c>
       <c r="T38" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="U38">
         <v>7.3339999999999996</v>
@@ -12214,8 +12260,8 @@
       <c r="A39">
         <v>25</v>
       </c>
-      <c r="B39" t="s">
-        <v>44</v>
+      <c r="B39" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="C39">
         <v>4.2439999999999998</v>
@@ -12239,7 +12285,7 @@
         <v>25</v>
       </c>
       <c r="K39" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="L39">
         <v>5.6669999999999998</v>
@@ -12263,7 +12309,7 @@
         <v>25</v>
       </c>
       <c r="T39" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="U39">
         <v>7.3570000000000002</v>
@@ -12374,7 +12420,7 @@
       <c r="A41">
         <v>27</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C41">
@@ -12399,7 +12445,7 @@
         <v>27</v>
       </c>
       <c r="K41" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="L41">
         <v>5.6669999999999998</v>
@@ -12423,7 +12469,7 @@
         <v>27</v>
       </c>
       <c r="T41" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="U41" t="s">
         <v>30</v>
@@ -12474,8 +12520,8 @@
       <c r="A42">
         <v>28</v>
       </c>
-      <c r="B42" t="s">
-        <v>51</v>
+      <c r="B42" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="C42">
         <v>4.2610000000000001</v>
@@ -12499,7 +12545,7 @@
         <v>28</v>
       </c>
       <c r="K42" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="L42">
         <v>5.6609999999999996</v>
@@ -12523,7 +12569,7 @@
         <v>28</v>
       </c>
       <c r="T42" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="U42">
         <v>7.3739999999999997</v>
@@ -12574,8 +12620,8 @@
       <c r="A43">
         <v>29</v>
       </c>
-      <c r="B43" t="s">
-        <v>53</v>
+      <c r="B43" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="C43">
         <v>4.2640000000000002</v>
@@ -12599,7 +12645,7 @@
         <v>29</v>
       </c>
       <c r="K43" t="s">
-        <v>53</v>
+        <v>136</v>
       </c>
       <c r="L43">
         <v>5.6740000000000004</v>
@@ -12623,7 +12669,7 @@
         <v>29</v>
       </c>
       <c r="T43" t="s">
-        <v>53</v>
+        <v>136</v>
       </c>
       <c r="U43">
         <v>7.3869999999999996</v>
@@ -12675,8 +12721,8 @@
       <c r="A44">
         <v>30</v>
       </c>
-      <c r="B44" t="s">
-        <v>54</v>
+      <c r="B44" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="C44">
         <v>4.2709999999999999</v>
@@ -12700,7 +12746,7 @@
         <v>30</v>
       </c>
       <c r="K44" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="L44">
         <v>5.6870000000000003</v>
@@ -12724,7 +12770,7 @@
         <v>30</v>
       </c>
       <c r="T44" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="U44" t="s">
         <v>30</v>
@@ -12775,8 +12821,8 @@
       <c r="A45">
         <v>31</v>
       </c>
-      <c r="B45" t="s">
-        <v>66</v>
+      <c r="B45" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="C45">
         <v>4.2640000000000002</v>
@@ -12800,7 +12846,7 @@
         <v>31</v>
       </c>
       <c r="K45" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="L45">
         <v>5.6769999999999996</v>
@@ -12824,7 +12870,7 @@
         <v>31</v>
       </c>
       <c r="T45" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="U45" t="s">
         <v>30</v>
@@ -13280,8 +13326,8 @@
       <c r="A50">
         <v>36</v>
       </c>
-      <c r="B50" t="s">
-        <v>60</v>
+      <c r="B50" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="C50">
         <v>4.2539999999999996</v>
@@ -13305,7 +13351,7 @@
         <v>36</v>
       </c>
       <c r="K50" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="L50">
         <v>5.6669999999999998</v>
@@ -13329,7 +13375,7 @@
         <v>36</v>
       </c>
       <c r="T50" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="U50">
         <v>7.3639999999999999</v>
@@ -13454,8 +13500,8 @@
       <c r="A52">
         <v>38</v>
       </c>
-      <c r="B52" t="s">
-        <v>43</v>
+      <c r="B52" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="C52">
         <v>4.2569999999999997</v>
@@ -13479,7 +13525,7 @@
         <v>38</v>
       </c>
       <c r="K52" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="L52">
         <v>5.6710000000000003</v>
@@ -13503,7 +13549,7 @@
         <v>38</v>
       </c>
       <c r="T52" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="U52">
         <v>7.3470000000000004</v>
@@ -13540,8 +13586,8 @@
       <c r="A53">
         <v>39</v>
       </c>
-      <c r="B53" t="s">
-        <v>44</v>
+      <c r="B53" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="C53">
         <v>4.2539999999999996</v>
@@ -13565,7 +13611,7 @@
         <v>39</v>
       </c>
       <c r="K53" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="L53">
         <v>5.6740000000000004</v>
@@ -13589,7 +13635,7 @@
         <v>39</v>
       </c>
       <c r="T53" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="U53">
         <v>7.367</v>

</xml_diff>